<commit_message>
refined 'working with time series data'
</commit_message>
<xml_diff>
--- a/Langtermyn-Koue Bokkeveld.xlsx
+++ b/Langtermyn-Koue Bokkeveld.xlsx
@@ -725,10 +725,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0630367667695762"/>
-          <c:y val="0.166417165668663"/>
-          <c:w val="0.910075778838058"/>
-          <c:h val="0.695109780439122"/>
+          <c:x val="0.0630403053777927"/>
+          <c:y val="0.166437928883344"/>
+          <c:w val="0.910014595262153"/>
+          <c:h val="0.695071740486588"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1099,11 +1099,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="1905085"/>
-        <c:axId val="20920904"/>
+        <c:axId val="19942725"/>
+        <c:axId val="621859"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1905085"/>
+        <c:axId val="19942725"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,14 +1145,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20920904"/>
+        <c:crossAx val="621859"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20920904"/>
+        <c:axId val="621859"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1194,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1905085"/>
+        <c:crossAx val="19942725"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,10 +1232,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0900479278263321"/>
-          <c:y val="0.038087835211815"/>
-          <c:w val="0.756413870876797"/>
-          <c:h val="0.759327633113098"/>
+          <c:x val="0.090053005526108"/>
+          <c:y val="0.038091536293849"/>
+          <c:w val="0.756343746475696"/>
+          <c:h val="0.759207074142455"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1445,8 +1445,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="10438880"/>
-        <c:axId val="29759567"/>
+        <c:axId val="84108332"/>
+        <c:axId val="80289224"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1655,11 +1655,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="50847860"/>
-        <c:axId val="58099097"/>
+        <c:axId val="60822770"/>
+        <c:axId val="65724078"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10438880"/>
+        <c:axId val="84108332"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,14 +1701,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29759567"/>
+        <c:crossAx val="80289224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29759567"/>
+        <c:axId val="80289224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,12 +1750,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10438880"/>
+        <c:crossAx val="84108332"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="50847860"/>
+        <c:axId val="60822770"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,14 +1787,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58099097"/>
+        <c:crossAx val="65724078"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58099097"/>
+        <c:axId val="65724078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1826,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50847860"/>
+        <c:crossAx val="60822770"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1896,9 +1896,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>354600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1907,7 +1907,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7279560" y="209160"/>
-        <a:ext cx="6413040" cy="2885400"/>
+        <a:ext cx="6412680" cy="2885040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1926,9 +1926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>418320</xdr:colOff>
+      <xdr:colOff>417960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1937,7 +1937,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7372080" y="3428640"/>
-        <a:ext cx="6384240" cy="3704760"/>
+        <a:ext cx="6383880" cy="3704400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1958,12 +1958,19 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="3.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Compacted working with time series data
</commit_message>
<xml_diff>
--- a/Langtermyn-Koue Bokkeveld.xlsx
+++ b/Langtermyn-Koue Bokkeveld.xlsx
@@ -504,9 +504,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -594,7 +595,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,6 +605,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,7 +684,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -725,10 +730,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0630403053777927"/>
-          <c:y val="0.166437928883344"/>
-          <c:w val="0.910014595262153"/>
-          <c:h val="0.695071740486588"/>
+          <c:x val="0.0630438443833156"/>
+          <c:y val="0.16645869727976"/>
+          <c:w val="0.909953404816707"/>
+          <c:h val="0.695033691040679"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1099,11 +1104,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19942725"/>
-        <c:axId val="621859"/>
+        <c:axId val="78899041"/>
+        <c:axId val="89157350"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19942725"/>
+        <c:axId val="78899041"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,14 +1150,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="621859"/>
+        <c:crossAx val="89157350"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="621859"/>
+        <c:axId val="89157350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1199,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19942725"/>
+        <c:crossAx val="78899041"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1221,7 +1226,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1232,10 +1237,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.090053005526108"/>
-          <c:y val="0.038091536293849"/>
-          <c:w val="0.756343746475696"/>
-          <c:h val="0.759207074142455"/>
+          <c:x val="0.0900580837985676"/>
+          <c:y val="0.0380952380952381"/>
+          <c:w val="0.75627361416568"/>
+          <c:h val="0.759086491739553"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1445,8 +1450,8 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="84108332"/>
-        <c:axId val="80289224"/>
+        <c:axId val="37498502"/>
+        <c:axId val="81744794"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1655,11 +1660,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60822770"/>
-        <c:axId val="65724078"/>
+        <c:axId val="46332155"/>
+        <c:axId val="90636866"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84108332"/>
+        <c:axId val="37498502"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,14 +1706,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80289224"/>
+        <c:crossAx val="81744794"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80289224"/>
+        <c:axId val="81744794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,12 +1755,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84108332"/>
+        <c:crossAx val="37498502"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="60822770"/>
+        <c:axId val="46332155"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,14 +1792,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65724078"/>
+        <c:crossAx val="90636866"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65724078"/>
+        <c:axId val="90636866"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1831,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60822770"/>
+        <c:crossAx val="46332155"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,16 +1894,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69120</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>-5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>543960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1906,8 +1911,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7279560" y="209160"/>
-        <a:ext cx="6412680" cy="2885040"/>
+        <a:off x="5060160" y="-5760"/>
+        <a:ext cx="11098440" cy="3420360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1926,9 +1931,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>417960</xdr:colOff>
+      <xdr:colOff>417600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1937,7 +1942,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7372080" y="3428640"/>
-        <a:ext cx="6383880" cy="3704400"/>
+        <a:ext cx="6383520" cy="3704040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1957,7 +1962,7 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -2980,17 +2985,17 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -2998,7 +3003,7 @@
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3007,7 +3012,7 @@
       <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3015,7 +3020,7 @@
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -3025,7 +3030,7 @@
         <f aca="false">C2*7</f>
         <v>16.1</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <f aca="false">D2/1768.9</f>
         <v>0.00910170162247724</v>
       </c>
@@ -3034,7 +3039,7 @@
       <c r="A3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -3045,7 +3050,7 @@
         <f aca="false">C3*7</f>
         <v>32.2</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <f aca="false">D3/1768.9</f>
         <v>0.0182034032449545</v>
       </c>
@@ -3054,7 +3059,7 @@
       <c r="A4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -3065,7 +3070,7 @@
         <f aca="false">C4*7</f>
         <v>48.3</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <f aca="false">D4/1768.9</f>
         <v>0.0273051048674317</v>
       </c>
@@ -3074,7 +3079,7 @@
       <c r="A5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -3085,7 +3090,7 @@
         <f aca="false">C5*7</f>
         <v>64.4</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <f aca="false">D5/1768.9</f>
         <v>0.036406806489909</v>
       </c>
@@ -3094,7 +3099,7 @@
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -3105,7 +3110,7 @@
         <f aca="false">C6*7</f>
         <v>80.5</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <f aca="false">D6/1768.9</f>
         <v>0.0455085081123862</v>
       </c>
@@ -3114,7 +3119,7 @@
       <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -3125,7 +3130,7 @@
         <f aca="false">C7*7</f>
         <v>97.3</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <f aca="false">D7/1768.9</f>
         <v>0.0550059358923625</v>
       </c>
@@ -3134,7 +3139,7 @@
       <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>2.5</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -3145,7 +3150,7 @@
         <f aca="false">C8*7</f>
         <v>114.8</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="3" t="n">
         <f aca="false">D8/1768.9</f>
         <v>0.0648990898298377</v>
       </c>
@@ -3154,7 +3159,7 @@
       <c r="A9" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>2.65</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -3165,7 +3170,7 @@
         <f aca="false">C9*7</f>
         <v>133.35</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="3" t="n">
         <f aca="false">D9/1768.9</f>
         <v>0.0753858330035615</v>
       </c>
@@ -3174,7 +3179,7 @@
       <c r="A10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="2" t="n">
         <v>2.8</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -3185,7 +3190,7 @@
         <f aca="false">C10*7</f>
         <v>152.95</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="3" t="n">
         <f aca="false">D10/1768.9</f>
         <v>0.0864661654135338</v>
       </c>
@@ -3194,7 +3199,7 @@
       <c r="A11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="2" t="n">
         <v>3.1</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -3205,7 +3210,7 @@
         <f aca="false">C11*7</f>
         <v>174.65</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <f aca="false">D11/1768.9</f>
         <v>0.0987336762960032</v>
       </c>
@@ -3214,7 +3219,7 @@
       <c r="A12" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="2" t="n">
         <v>3.4</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -3225,7 +3230,7 @@
         <f aca="false">C12*7</f>
         <v>198.45</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="3" t="n">
         <f aca="false">D12/1768.9</f>
         <v>0.11218836565097</v>
       </c>
@@ -3234,7 +3239,7 @@
       <c r="A13" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="2" t="n">
         <v>3.65</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -3245,7 +3250,7 @@
         <f aca="false">C13*7</f>
         <v>224</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="3" t="n">
         <f aca="false">D13/1768.9</f>
         <v>0.126632370399683</v>
       </c>
@@ -3254,7 +3259,7 @@
       <c r="A14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="2" t="n">
         <v>4</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -3265,7 +3270,7 @@
         <f aca="false">C14*7</f>
         <v>252</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="3" t="n">
         <f aca="false">D14/1768.9</f>
         <v>0.142461416699644</v>
       </c>
@@ -3274,7 +3279,7 @@
       <c r="A15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="2" t="n">
         <v>4.4</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -3285,7 +3290,7 @@
         <f aca="false">C15*7</f>
         <v>282.8</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="3" t="n">
         <f aca="false">D15/1768.9</f>
         <v>0.1598733676296</v>
       </c>
@@ -3294,7 +3299,7 @@
       <c r="A16" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="2" t="n">
         <v>4.8</v>
       </c>
       <c r="C16" s="1" t="n">
@@ -3305,7 +3310,7 @@
         <f aca="false">C16*7</f>
         <v>316.4</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="3" t="n">
         <f aca="false">D16/1768.9</f>
         <v>0.178868223189553</v>
       </c>
@@ -3314,7 +3319,7 @@
       <c r="A17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="2" t="n">
         <v>5.3</v>
       </c>
       <c r="C17" s="1" t="n">
@@ -3325,7 +3330,7 @@
         <f aca="false">C17*7</f>
         <v>353.5</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="3" t="n">
         <f aca="false">D17/1768.9</f>
         <v>0.199841709537</v>
       </c>
@@ -3334,7 +3339,7 @@
       <c r="A18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="2" t="n">
         <v>5.8</v>
       </c>
       <c r="C18" s="1" t="n">
@@ -3345,7 +3350,7 @@
         <f aca="false">C18*7</f>
         <v>394.1</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="3" t="n">
         <f aca="false">D18/1768.9</f>
         <v>0.222793826671943</v>
       </c>
@@ -3354,7 +3359,7 @@
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" s="2" t="n">
         <v>6.3</v>
       </c>
       <c r="C19" s="1" t="n">
@@ -3365,7 +3370,7 @@
         <f aca="false">C19*7</f>
         <v>438.2</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="3" t="n">
         <f aca="false">D19/1768.9</f>
         <v>0.247724574594381</v>
       </c>
@@ -3374,7 +3379,7 @@
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" s="2" t="n">
         <v>6.7</v>
       </c>
       <c r="C20" s="1" t="n">
@@ -3385,7 +3390,7 @@
         <f aca="false">C20*7</f>
         <v>485.1</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="3" t="n">
         <f aca="false">D20/1768.9</f>
         <v>0.274238227146814</v>
       </c>
@@ -3394,7 +3399,7 @@
       <c r="A21" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" s="2" t="n">
         <v>7.1</v>
       </c>
       <c r="C21" s="1" t="n">
@@ -3405,7 +3410,7 @@
         <f aca="false">C21*7</f>
         <v>534.8</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="3" t="n">
         <f aca="false">D21/1768.9</f>
         <v>0.302334784329244</v>
       </c>
@@ -3414,7 +3419,7 @@
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" s="2" t="n">
         <v>7.6</v>
       </c>
       <c r="C22" s="1" t="n">
@@ -3425,7 +3430,7 @@
         <f aca="false">C22*7</f>
         <v>588</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="3" t="n">
         <f aca="false">D22/1768.9</f>
         <v>0.332409972299169</v>
       </c>
@@ -3434,7 +3439,7 @@
       <c r="A23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" s="2" t="n">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -3445,7 +3450,7 @@
         <f aca="false">C23*7</f>
         <v>644</v>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="3" t="n">
         <f aca="false">D23/1768.9</f>
         <v>0.36406806489909</v>
       </c>
@@ -3454,7 +3459,7 @@
       <c r="A24" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="2" t="n">
         <v>8.3</v>
       </c>
       <c r="C24" s="1" t="n">
@@ -3465,7 +3470,7 @@
         <f aca="false">C24*7</f>
         <v>702.1</v>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="3" t="n">
         <f aca="false">D24/1768.9</f>
         <v>0.396913335971508</v>
       </c>
@@ -3474,7 +3479,7 @@
       <c r="A25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="2" t="n">
         <v>8.6</v>
       </c>
       <c r="C25" s="1" t="n">
@@ -3485,7 +3490,7 @@
         <f aca="false">C25*7</f>
         <v>762.3</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="3" t="n">
         <f aca="false">D25/1768.9</f>
         <v>0.430945785516423</v>
       </c>
@@ -3494,7 +3499,7 @@
       <c r="A26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" s="2" t="n">
         <v>8.8</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -3505,7 +3510,7 @@
         <f aca="false">C26*7</f>
         <v>823.9</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="3" t="n">
         <f aca="false">D26/1768.9</f>
         <v>0.465769687376335</v>
       </c>
@@ -3514,7 +3519,7 @@
       <c r="A27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="2" t="n">
         <v>8.9</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -3525,7 +3530,7 @@
         <f aca="false">C27*7</f>
         <v>886.2</v>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="3" t="n">
         <f aca="false">D27/1768.9</f>
         <v>0.500989315393747</v>
       </c>
@@ -3534,7 +3539,7 @@
       <c r="A28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="2" t="n">
         <v>8.9</v>
       </c>
       <c r="C28" s="1" t="n">
@@ -3545,7 +3550,7 @@
         <f aca="false">C28*7</f>
         <v>948.5</v>
       </c>
-      <c r="E28" s="2" t="n">
+      <c r="E28" s="3" t="n">
         <f aca="false">D28/1768.9</f>
         <v>0.536208943411159</v>
       </c>
@@ -3554,7 +3559,7 @@
       <c r="A29" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="2" t="n">
         <v>8.9</v>
       </c>
       <c r="C29" s="1" t="n">
@@ -3565,7 +3570,7 @@
         <f aca="false">C29*7</f>
         <v>1010.8</v>
       </c>
-      <c r="E29" s="2" t="n">
+      <c r="E29" s="3" t="n">
         <f aca="false">D29/1768.9</f>
         <v>0.571428571428571</v>
       </c>
@@ -3574,7 +3579,7 @@
       <c r="A30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="2" t="n">
         <v>8.8</v>
       </c>
       <c r="C30" s="1" t="n">
@@ -3585,7 +3590,7 @@
         <f aca="false">C30*7</f>
         <v>1072.4</v>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="3" t="n">
         <f aca="false">D30/1768.9</f>
         <v>0.606252473288484</v>
       </c>
@@ -3594,7 +3599,7 @@
       <c r="A31" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>8.7</v>
       </c>
       <c r="C31" s="1" t="n">
@@ -3605,7 +3610,7 @@
         <f aca="false">C31*7</f>
         <v>1133.3</v>
       </c>
-      <c r="E31" s="2" t="n">
+      <c r="E31" s="3" t="n">
         <f aca="false">D31/1768.9</f>
         <v>0.640680648990898</v>
       </c>
@@ -3614,7 +3619,7 @@
       <c r="A32" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="2" t="n">
         <v>8.5</v>
       </c>
       <c r="C32" s="1" t="n">
@@ -3625,7 +3630,7 @@
         <f aca="false">C32*7</f>
         <v>1192.8</v>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="3" t="n">
         <f aca="false">D32/1768.9</f>
         <v>0.674317372378314</v>
       </c>
@@ -3634,7 +3639,7 @@
       <c r="A33" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="2" t="n">
         <v>8.3</v>
       </c>
       <c r="C33" s="1" t="n">
@@ -3645,7 +3650,7 @@
         <f aca="false">C33*7</f>
         <v>1250.9</v>
       </c>
-      <c r="E33" s="2" t="n">
+      <c r="E33" s="3" t="n">
         <f aca="false">D33/1768.9</f>
         <v>0.707162643450732</v>
       </c>
@@ -3654,7 +3659,7 @@
       <c r="A34" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="2" t="n">
         <v>8</v>
       </c>
       <c r="C34" s="1" t="n">
@@ -3665,7 +3670,7 @@
         <f aca="false">C34*7</f>
         <v>1306.9</v>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" s="3" t="n">
         <f aca="false">D34/1768.9</f>
         <v>0.738820736050653</v>
       </c>
@@ -3674,7 +3679,7 @@
       <c r="A35" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="2" t="n">
         <v>7.5</v>
       </c>
       <c r="C35" s="1" t="n">
@@ -3685,7 +3690,7 @@
         <f aca="false">C35*7</f>
         <v>1359.4</v>
       </c>
-      <c r="E35" s="2" t="n">
+      <c r="E35" s="3" t="n">
         <f aca="false">D35/1768.9</f>
         <v>0.768500197863079</v>
       </c>
@@ -3694,7 +3699,7 @@
       <c r="A36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="2" t="n">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="n">
@@ -3705,7 +3710,7 @@
         <f aca="false">C36*7</f>
         <v>1408.4</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="3" t="n">
         <f aca="false">D36/1768.9</f>
         <v>0.796201028888009</v>
       </c>
@@ -3714,7 +3719,7 @@
       <c r="A37" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="2" t="n">
         <v>6.5</v>
       </c>
       <c r="C37" s="1" t="n">
@@ -3725,7 +3730,7 @@
         <f aca="false">C37*7</f>
         <v>1453.9</v>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="3" t="n">
         <f aca="false">D37/1768.9</f>
         <v>0.821923229125445</v>
       </c>
@@ -3734,7 +3739,7 @@
       <c r="A38" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="2" t="n">
         <v>5.8</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -3745,7 +3750,7 @@
         <f aca="false">C38*7</f>
         <v>1494.5</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="3" t="n">
         <f aca="false">D38/1768.9</f>
         <v>0.844875346260388</v>
       </c>
@@ -3754,7 +3759,7 @@
       <c r="A39" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="2" t="n">
         <v>5.2</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -3765,7 +3770,7 @@
         <f aca="false">C39*7</f>
         <v>1530.9</v>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="3" t="n">
         <f aca="false">D39/1768.9</f>
         <v>0.865453106450336</v>
       </c>
@@ -3774,7 +3779,7 @@
       <c r="A40" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="2" t="n">
         <v>4.7</v>
       </c>
       <c r="C40" s="1" t="n">
@@ -3785,7 +3790,7 @@
         <f aca="false">C40*7</f>
         <v>1563.8</v>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="3" t="n">
         <f aca="false">D40/1768.9</f>
         <v>0.88405223585279</v>
       </c>
@@ -3794,7 +3799,7 @@
       <c r="A41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="2" t="n">
         <v>4.3</v>
       </c>
       <c r="C41" s="1" t="n">
@@ -3805,7 +3810,7 @@
         <f aca="false">C41*7</f>
         <v>1593.9</v>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="3" t="n">
         <f aca="false">D41/1768.9</f>
         <v>0.901068460625247</v>
       </c>
@@ -3814,7 +3819,7 @@
       <c r="A42" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="2" t="n">
         <v>3.7</v>
       </c>
       <c r="C42" s="1" t="n">
@@ -3825,7 +3830,7 @@
         <f aca="false">C42*7</f>
         <v>1619.8</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="3" t="n">
         <f aca="false">D42/1768.9</f>
         <v>0.915710328452711</v>
       </c>
@@ -3834,7 +3839,7 @@
       <c r="A43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="2" t="n">
         <v>3.4</v>
       </c>
       <c r="C43" s="1" t="n">
@@ -3845,7 +3850,7 @@
         <f aca="false">C43*7</f>
         <v>1643.6</v>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="3" t="n">
         <f aca="false">D43/1768.9</f>
         <v>0.929165017807677</v>
       </c>
@@ -3854,7 +3859,7 @@
       <c r="A44" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="2" t="n">
         <v>3.1</v>
       </c>
       <c r="C44" s="1" t="n">
@@ -3865,7 +3870,7 @@
         <f aca="false">C44*7</f>
         <v>1665.3</v>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="3" t="n">
         <f aca="false">D44/1768.9</f>
         <v>0.941432528690146</v>
       </c>
@@ -3874,7 +3879,7 @@
       <c r="A45" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="2" t="n">
         <v>2.8</v>
       </c>
       <c r="C45" s="1" t="n">
@@ -3885,7 +3890,7 @@
         <f aca="false">C45*7</f>
         <v>1684.9</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="3" t="n">
         <f aca="false">D45/1768.9</f>
         <v>0.952512861100118</v>
       </c>
@@ -3894,7 +3899,7 @@
       <c r="A46" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="2" t="n">
         <v>2.5</v>
       </c>
       <c r="C46" s="1" t="n">
@@ -3905,7 +3910,7 @@
         <f aca="false">C46*7</f>
         <v>1702.4</v>
       </c>
-      <c r="E46" s="2" t="n">
+      <c r="E46" s="3" t="n">
         <f aca="false">D46/1768.9</f>
         <v>0.962406015037594</v>
       </c>
@@ -3914,7 +3919,7 @@
       <c r="A47" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="2" t="n">
         <v>2.45</v>
       </c>
       <c r="C47" s="1" t="n">
@@ -3925,7 +3930,7 @@
         <f aca="false">C47*7</f>
         <v>1719.55</v>
       </c>
-      <c r="E47" s="2" t="n">
+      <c r="E47" s="3" t="n">
         <f aca="false">D47/1768.9</f>
         <v>0.972101305896319</v>
       </c>
@@ -3934,7 +3939,7 @@
       <c r="A48" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="2" t="n">
         <v>2.4</v>
       </c>
       <c r="C48" s="1" t="n">
@@ -3945,7 +3950,7 @@
         <f aca="false">C48*7</f>
         <v>1736.35</v>
       </c>
-      <c r="E48" s="2" t="n">
+      <c r="E48" s="3" t="n">
         <f aca="false">D48/1768.9</f>
         <v>0.981598733676296</v>
       </c>
@@ -3954,7 +3959,7 @@
       <c r="A49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="2" t="n">
         <v>2.35</v>
       </c>
       <c r="C49" s="1" t="n">
@@ -3965,7 +3970,7 @@
         <f aca="false">C49*7</f>
         <v>1752.8</v>
       </c>
-      <c r="E49" s="2" t="n">
+      <c r="E49" s="3" t="n">
         <f aca="false">D49/1768.9</f>
         <v>0.990898298377523</v>
       </c>
@@ -3974,7 +3979,7 @@
       <c r="A50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="B50" s="2" t="n">
         <v>2.3</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -3985,7 +3990,7 @@
         <f aca="false">C50*7</f>
         <v>1768.9</v>
       </c>
-      <c r="E50" s="2" t="n">
+      <c r="E50" s="3" t="n">
         <f aca="false">D50/1768.9</f>
         <v>1</v>
       </c>

</xml_diff>